<commit_message>
HTML tag sequence test
</commit_message>
<xml_diff>
--- a/reports/vacation_rental_test_results.xlsx
+++ b/reports/vacation_rental_test_results.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G8"/>
+  <dimension ref="A1:G25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -473,7 +473,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/</t>
+          <t>https://www.alojamiento.io/property/apartamentos-centro-col%c3%b3n/BC-189483</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -491,7 +491,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>2024-12-06 10:32:18</t>
+          <t>2024-12-06 17:44:12</t>
         </is>
       </c>
       <c r="F2" t="inlineStr"/>
@@ -502,7 +502,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/</t>
+          <t>https://www.alojamiento.io/property/apartamentos-centro-col%c3%b3n/BC-189483</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -520,7 +520,7 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>2024-12-06 10:44:51</t>
+          <t>2024-12-06 17:58:08</t>
         </is>
       </c>
       <c r="F3" t="n">
@@ -533,38 +533,36 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/</t>
+          <t>https://www.alojamiento.io/property/apartamentos-centro-col%c3%b3n/BC-189483</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>H1 Tag Existence</t>
+          <t>H1-H6 Tag Sequence</t>
         </is>
       </c>
       <c r="C4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>H1 tag found</t>
+          <t>H5 missing</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>2024-12-06 11:27:12</t>
-        </is>
-      </c>
-      <c r="F4" t="n">
-        <v>1</v>
-      </c>
+          <t>2024-12-06 17:58:08</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr"/>
       <c r="G4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/</t>
+          <t>https://www.alojamiento.io/property/apartamentos-centro-col%c3%b3n/BC-189483</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -582,7 +580,7 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>2024-12-06 16:17:43</t>
+          <t>2024-12-06 18:01:35</t>
         </is>
       </c>
       <c r="F5" t="n">
@@ -595,29 +593,29 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/</t>
+          <t>https://www.alojamiento.io/property/apartamentos-centro-col%c3%b3n/BC-189483</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>H1 Tag Existence</t>
+          <t>H1-H6 Tag Sequence</t>
         </is>
       </c>
       <c r="C6" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>H1 tag found</t>
+          <t>H5 missing</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>2024-12-06 16:20:05</t>
+          <t>2024-12-06 18:01:35</t>
         </is>
       </c>
       <c r="F6" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G6" t="b">
         <v>0</v>
@@ -626,7 +624,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/</t>
+          <t>https://www.alojamiento.io/property/apartamentos-centro-col%c3%b3n/BC-189483</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -644,7 +642,7 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>2024-12-06 16:22:21</t>
+          <t>2024-12-06 18:02:50</t>
         </is>
       </c>
       <c r="F7" t="n">
@@ -657,32 +655,549 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
+          <t>https://www.alojamiento.io/property/apartamentos-centro-col%c3%b3n/BC-189483</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>H1-H6 Tag Sequence</t>
+        </is>
+      </c>
+      <c r="C8" t="b">
+        <v>0</v>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>H5 missing</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>2024-12-06 18:02:50</t>
+        </is>
+      </c>
+      <c r="F8" t="n">
+        <v>0</v>
+      </c>
+      <c r="G8" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>https://www.alojamiento.io/property/apartamentos-centro-col%c3%b3n/BC-189483</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>H1 Tag Existence</t>
+        </is>
+      </c>
+      <c r="C9" t="b">
+        <v>1</v>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>H1 tag found</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>2024-12-06 18:03:52</t>
+        </is>
+      </c>
+      <c r="F9" t="n">
+        <v>1</v>
+      </c>
+      <c r="G9" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>https://www.alojamiento.io/property/apartamentos-centro-col%c3%b3n/BC-189483</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>H1-H6 Tag Sequence</t>
+        </is>
+      </c>
+      <c r="C10" t="b">
+        <v>0</v>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>H5 missing</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>2024-12-06 18:03:52</t>
+        </is>
+      </c>
+      <c r="F10" t="n">
+        <v>0</v>
+      </c>
+      <c r="G10" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>https://www.alojamiento.io/property/apartamentos-centro-col%c3%b3n/BC-189483</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>H1 Tag Existence</t>
+        </is>
+      </c>
+      <c r="C11" t="b">
+        <v>1</v>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>H1 tag found</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>2024-12-06 18:05:25</t>
+        </is>
+      </c>
+      <c r="F11" t="n">
+        <v>1</v>
+      </c>
+      <c r="G11" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>https://www.alojamiento.io/property/apartamentos-centro-col%c3%b3n/BC-189483</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>H1-H6 Tag Sequence</t>
+        </is>
+      </c>
+      <c r="C12" t="b">
+        <v>0</v>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>H5 missing</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>2024-12-06 18:05:25</t>
+        </is>
+      </c>
+      <c r="F12" t="n">
+        <v>0</v>
+      </c>
+      <c r="G12" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>https://www.alojamiento.io/property/apartamentos-centro-col%c3%b3n/BC-189483</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>H1 Tag Existence</t>
+        </is>
+      </c>
+      <c r="C13" t="b">
+        <v>1</v>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>H1 tag found</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>2024-12-06 18:08:48</t>
+        </is>
+      </c>
+      <c r="F13" t="n">
+        <v>1</v>
+      </c>
+      <c r="G13" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>https://www.alojamiento.io/property/apartamentos-centro-col%c3%b3n/BC-189483</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>H1-H6 Tag Sequence</t>
+        </is>
+      </c>
+      <c r="C14" t="b">
+        <v>1</v>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>Tags found in correct sequence</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>2024-12-06 18:08:48</t>
+        </is>
+      </c>
+      <c r="F14" t="n">
+        <v>0</v>
+      </c>
+      <c r="G14" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>https://www.alojamiento.io/property/consultar-disponibilidad/BC-4505653</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>H1 Tag Existence</t>
+        </is>
+      </c>
+      <c r="C15" t="b">
+        <v>1</v>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>H1 tag found</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>2024-12-06 18:11:51</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr"/>
+      <c r="G15" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>https://www.alojamiento.io/property/consultar-disponibilidad/BC-4505653</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>H1-H6 Tag Sequence</t>
+        </is>
+      </c>
+      <c r="C16" t="b">
+        <v>1</v>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>Tags found in correct sequence</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>2024-12-06 18:11:51</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr"/>
+      <c r="G16" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>https://www.alojamiento.io/property/consultar-disponibilidad/BC-4505653</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>H1 Tag Existence</t>
+        </is>
+      </c>
+      <c r="C17" t="b">
+        <v>1</v>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>H1 tag found</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>2024-12-06 18:13:42</t>
+        </is>
+      </c>
+      <c r="F17" t="n">
+        <v>1</v>
+      </c>
+      <c r="G17" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>https://www.alojamiento.io/property/consultar-disponibilidad/BC-4505653</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>H1-H6 Tag Sequence</t>
+        </is>
+      </c>
+      <c r="C18" t="b">
+        <v>1</v>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>Tags found in correct sequence</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>2024-12-06 18:13:42</t>
+        </is>
+      </c>
+      <c r="F18" t="n">
+        <v>1</v>
+      </c>
+      <c r="G18" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>https://www.alojamiento.io/property/bonita-casa-de-campo-t%C3%ADpica-mallorquina/BC-12224317</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>H1 Tag Existence</t>
+        </is>
+      </c>
+      <c r="C19" t="b">
+        <v>1</v>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>H1 tag found</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>2024-12-06 18:17:02</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr"/>
+      <c r="G19" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>https://www.alojamiento.io/property/bonita-casa-de-campo-t%C3%ADpica-mallorquina/BC-12224317</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>H1-H6 Tag Sequence</t>
+        </is>
+      </c>
+      <c r="C20" t="b">
+        <v>1</v>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>Tags found in correct sequence</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>2024-12-06 18:17:02</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr"/>
+      <c r="G20" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>https://www.alojamiento.io/property/bonita-casa-de-campo-t%C3%ADpica-mallorquina/BC-12224317</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>H1 Tag Existence</t>
+        </is>
+      </c>
+      <c r="C21" t="b">
+        <v>1</v>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>H1 tag found</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>2024-12-06 18:25:50</t>
+        </is>
+      </c>
+      <c r="F21" t="n">
+        <v>1</v>
+      </c>
+      <c r="G21" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
           <t>https://www.alojamiento.io/</t>
         </is>
       </c>
-      <c r="B8" t="inlineStr">
+      <c r="B22" t="inlineStr">
         <is>
           <t>H1 Tag Existence</t>
         </is>
       </c>
-      <c r="C8" t="b">
-        <v>1</v>
-      </c>
-      <c r="D8" t="inlineStr">
+      <c r="C22" t="b">
+        <v>1</v>
+      </c>
+      <c r="D22" t="inlineStr">
         <is>
           <t>H1 tag found</t>
         </is>
       </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>2024-12-06 16:38:47</t>
-        </is>
-      </c>
-      <c r="F8" t="n">
-        <v>1</v>
-      </c>
-      <c r="G8" t="b">
-        <v>0</v>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>2024-12-06 18:29:47</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr"/>
+      <c r="G22" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>https://www.alojamiento.io/</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>H1-H6 Tag Sequence</t>
+        </is>
+      </c>
+      <c r="C23" t="b">
+        <v>1</v>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>Tags found in correct sequence</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>2024-12-06 18:29:47</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr"/>
+      <c r="G23" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>https://www.alojamiento.io/</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>H1 Tag Existence</t>
+        </is>
+      </c>
+      <c r="C24" t="b">
+        <v>1</v>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>H1 tag found</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>2024-12-06 18:32:30</t>
+        </is>
+      </c>
+      <c r="F24" t="b">
+        <v>1</v>
+      </c>
+      <c r="G24" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>https://www.alojamiento.io/</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>HTML Tag Sequence</t>
+        </is>
+      </c>
+      <c r="C25" t="b">
+        <v>0</v>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>Improper heading hierarchy</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>2024-12-06 18:32:30</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="G25" t="b">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>